<commit_message>
feat：mainUI change and delete light dragon
</commit_message>
<xml_diff>
--- a/Excels/Task_小游戏任务表.xlsx
+++ b/Excels/Task_小游戏任务表.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MetaApp\Editor_Win64\MetaWorldSaved\Saved\MetaWorld\Project\Edit\DragonVerse\Excels\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5F6FBA-5744-463D-88E0-A2837160E392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="24045" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>int</t>
   </si>
@@ -73,24 +80,36 @@
     <t>获取木龙</t>
   </si>
   <si>
+    <t>34|1|1||35|1|1||36|1|1||37|1|1||38|1|1</t>
+  </si>
+  <si>
     <t>BFA2FBF640BDA222EEB4B9884B78C1B4</t>
   </si>
   <si>
     <t>获取火龙</t>
   </si>
   <si>
+    <t>24|1|1||25|1|1||26|1|1||27|1|1||28|1|1</t>
+  </si>
+  <si>
     <t>0B777B1642A1212E59FA3DA8648142A7</t>
   </si>
   <si>
     <t>获取水龙</t>
   </si>
   <si>
+    <t>29|1|1||30|1|1||31|1|1||32|1|1||33|1|1</t>
+  </si>
+  <si>
     <t>1BF851F4459908F9C2AAB884763B1750</t>
   </si>
   <si>
     <t>获取土龙</t>
   </si>
   <si>
+    <t>39|1|1||41|1|1||42|1|1||43|1|1||44|1|1</t>
+  </si>
+  <si>
     <t>D759B111445E9ECDC60E0EB67C073831</t>
   </si>
   <si>
@@ -98,73 +117,376 @@
   </si>
   <si>
     <t>0F362B364C669123BC0886AEC93884B0</t>
-  </si>
-  <si>
-    <t>光暗龙</t>
-  </si>
-  <si>
-    <t>7949884C461020935235E5834F66108F</t>
-  </si>
-  <si>
-    <t>34|1|1||35|1|1||36|1|1||37|1|1||38|1|1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>29|1|1||30|1|1||31|1|1||32|1|1||33|1|1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>39|1|1||41|1|1||42|1|1||43|1|1||44|1|1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>45|1|1||46|1|1||47|1|1||48|1|1||49|1|1||50|1|1||51|1|1||52|1|1||53|1|1||54|1|1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>24|1|1||25|1|1||26|1|1||27|1|1||28|1|1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="10"/>
-      <color indexed="64"/>
-      <name val="微软雅黑"/>
-    </font>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="64"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -172,17 +494,259 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -199,28 +763,69 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="">
       <a:dk1>
@@ -272,7 +877,7 @@
         <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme>
+    <a:fmtScheme name="">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -387,29 +992,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16.5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="46.75" customWidth="1"/>
     <col min="2" max="2" width="51.875" customWidth="1"/>
-    <col min="3" max="3" width="51.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.875" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.125" customWidth="1"/>
-    <col min="5" max="5" width="61" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61" customWidth="1"/>
     <col min="6" max="6" width="35.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" s="1" customFormat="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -419,17 +1024,17 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" s="1" customFormat="1" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -439,38 +1044,38 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="3" s="1" customFormat="1" ht="72.75" customHeight="1" spans="1:6">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" s="2" customFormat="1"/>
+    <row r="5" s="2" customFormat="1" spans="1:6">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -480,116 +1085,101 @@
       <c r="C5" s="6">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="1:6">
+      <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C6" s="6">
         <v>6</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" spans="1:6">
       <c r="A7" s="5">
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="6">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+      <c r="E7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="1" spans="1:6">
+      <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+      <c r="E8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" s="2" customFormat="1" spans="1:6">
+      <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" spans="3:5">
+      <c r="C10" s="6"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" s="2" customFormat="1"/>
+    <row r="12" s="2" customFormat="1"/>
+    <row r="13" s="2" customFormat="1" spans="3:8">
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -597,42 +1187,42 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" s="2" customFormat="1" spans="4:8">
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" s="2" customFormat="1" spans="4:8">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" s="2" customFormat="1" spans="4:8">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" s="2" customFormat="1" spans="4:8">
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" s="2" customFormat="1" spans="4:8">
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" s="2" customFormat="1" spans="1:8">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="6"/>
@@ -642,7 +1232,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" s="2" customFormat="1" spans="1:8">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="6"/>
@@ -652,109 +1242,108 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" s="2" customFormat="1" spans="1:2">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" s="2" customFormat="1" spans="1:2">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" s="2" customFormat="1" spans="1:2">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" s="2" customFormat="1" spans="1:2">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" s="2" customFormat="1" spans="1:2">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
     </row>
-    <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" s="2" customFormat="1" spans="1:3">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" s="2" customFormat="1" spans="1:3">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" s="2" customFormat="1" spans="1:2">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
     </row>
-    <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" s="2" customFormat="1" spans="1:2">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" s="2" customFormat="1" spans="1:2">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" s="2" customFormat="1" spans="1:2">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" s="2" customFormat="1" spans="1:2">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
     </row>
-    <row r="33" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" s="2" customFormat="1" spans="1:2">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" s="2" customFormat="1" spans="1:2">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
     </row>
-    <row r="35" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" s="2" customFormat="1" spans="1:2">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
     </row>
-    <row r="36" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" s="2" customFormat="1" spans="1:2">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
     </row>
-    <row r="37" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" s="2" customFormat="1" spans="1:2">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
     </row>
-    <row r="38" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" s="2" customFormat="1" spans="1:2">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" s="2" customFormat="1" spans="1:2">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" s="2" customFormat="1" spans="1:2">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
     </row>
-    <row r="41" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" s="2" customFormat="1" spans="1:2">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
     </row>
-    <row r="42" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" s="2" customFormat="1" spans="1:2">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
     </row>
-    <row r="43" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" s="2" customFormat="1" spans="1:2">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
     </row>
-    <row r="44" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" s="2" customFormat="1" spans="1:2">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
     </row>
-    <row r="45" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="45" s="2" customFormat="1"/>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.0249999999999997" bottom="1.0249999999999997" header="0.78750000000000009" footer="0.78750000000000009"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,标准"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,标准"页 &amp;P</oddFooter>

</xml_diff>

<commit_message>
feat:light and dark dragon change
</commit_message>
<xml_diff>
--- a/Excels/Task_小游戏任务表.xlsx
+++ b/Excels/Task_小游戏任务表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>int</t>
   </si>
@@ -107,10 +107,19 @@
     <t>获取土龙</t>
   </si>
   <si>
-    <t>39|1|1||41|1|1||42|1|1||43|1|1||44|1|1</t>
+    <t>39|1|1||40|1|1||41|1|1||42|1|1||43|1|1</t>
   </si>
   <si>
     <t>D759B111445E9ECDC60E0EB67C073831</t>
+  </si>
+  <si>
+    <t>获取光暗龙</t>
+  </si>
+  <si>
+    <t>44|1|1||45|1|1||46|1|1||47|1|1||48|1|1||49|1|1||50|1|1||51|1|1||52|1|1||53|1|1</t>
+  </si>
+  <si>
+    <t>7949884C461020935235E5834F66108F</t>
   </si>
   <si>
     <t>跑酷</t>
@@ -129,12 +138,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
-    <font>
-      <sz val="10"/>
-      <name val="微软雅黑"/>
-      <charset val="134"/>
-    </font>
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -595,148 +599,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -748,19 +752,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1000,8 +1004,8 @@
   <sheetPr/>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16.5" outlineLevelCol="7"/>
@@ -1168,14 +1172,29 @@
       <c r="D9" s="2">
         <v>0</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" s="2" customFormat="1" spans="3:5">
-      <c r="C10" s="6"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="7"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" spans="1:6">
+      <c r="A10" s="2">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" s="2" customFormat="1"/>
     <row r="12" s="2" customFormat="1"/>

</xml_diff>